<commit_message>
Fix EQ5D02 collection DS
</commit_message>
<xml_diff>
--- a/curation/draft/collection/collection_specialization_QRS_EQ5D-5L.xlsx
+++ b/curation/draft/collection/collection_specialization_QRS_EQ5D-5L.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\cdisc-org\COSMoS\curation\draft\collection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B34C81EB-91E4-43D2-810D-8488F6180356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAED1C6A-0F3F-4CF6-A767-EE7F78350A68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Collection_QRS_EQ5D-5L'!$A$1:$AG$16</definedName>
   </definedNames>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="157">
   <si>
     <t>package_date</t>
   </si>
@@ -689,7 +689,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -733,7 +733,6 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1039,10 +1038,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="T1" sqref="T1"/>
-      <selection pane="bottomLeft" activeCell="O12" sqref="O12"/>
+      <selection pane="bottomLeft" activeCell="V5" sqref="V5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1404,9 +1403,6 @@
       <c r="T5">
         <v>5</v>
       </c>
-      <c r="V5" t="s">
-        <v>33</v>
-      </c>
       <c r="Z5"/>
       <c r="AB5" s="5" t="s">
         <v>48</v>
@@ -1815,7 +1811,7 @@
       <c r="M12" t="s">
         <v>65</v>
       </c>
-      <c r="N12" s="19" t="s">
+      <c r="N12" t="s">
         <v>156</v>
       </c>
       <c r="P12" s="4" t="s">

</xml_diff>

<commit_message>
EQ5D-5L updated to include categories
</commit_message>
<xml_diff>
--- a/curation/draft/collection/collection_specialization_QRS_EQ5D-5L.xlsx
+++ b/curation/draft/collection/collection_specialization_QRS_EQ5D-5L.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\cdisc-org\COSMoS\curation\draft\collection\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dagmarkottig/COSMoS/curation/draft/collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF1187BD-E457-48D6-B5AD-206F56B96D11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E99F4A4-9707-9443-AE3D-747E05D96961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="915" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4300" yWindow="780" windowWidth="29900" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Collection_QRS_EQ5D-5L" sheetId="1" r:id="rId1"/>
     <sheet name="FORM_QRS_EQ5D-5L" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Collection_QRS_EQ5D-5L'!$A$1:$AG$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Collection_QRS_EQ5D-5L'!$A$1:$AH$16</definedName>
   </definedNames>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="165">
   <si>
     <t>package_date</t>
   </si>
@@ -535,12 +535,15 @@
   <si>
     <t>EQ5D02_QSEVINTX</t>
   </si>
+  <si>
+    <t>categories</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1057,47 +1060,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG16"/>
+  <dimension ref="A1:AH16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="T1" sqref="T1"/>
-      <selection pane="bottomLeft" activeCell="L6" sqref="L6"/>
+      <selection pane="bottomLeft" activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="19.42578125" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" customWidth="1"/>
-    <col min="8" max="8" width="25.42578125" customWidth="1"/>
-    <col min="9" max="9" width="19.7109375" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" customWidth="1"/>
-    <col min="11" max="11" width="28.7109375" customWidth="1"/>
-    <col min="12" max="12" width="19.42578125" customWidth="1"/>
-    <col min="13" max="13" width="12.140625" customWidth="1"/>
-    <col min="14" max="14" width="13.85546875" customWidth="1"/>
-    <col min="15" max="15" width="17.28515625" customWidth="1"/>
-    <col min="16" max="16" width="36.85546875" style="4" customWidth="1"/>
-    <col min="17" max="17" width="13" customWidth="1"/>
-    <col min="18" max="18" width="22.42578125" customWidth="1"/>
-    <col min="20" max="20" width="14" customWidth="1"/>
-    <col min="21" max="21" width="15.42578125" customWidth="1"/>
-    <col min="22" max="22" width="15" customWidth="1"/>
-    <col min="23" max="23" width="21.42578125" customWidth="1"/>
-    <col min="24" max="24" width="29.140625" customWidth="1"/>
-    <col min="25" max="25" width="52" customWidth="1"/>
-    <col min="26" max="26" width="47.7109375" style="4" customWidth="1"/>
-    <col min="27" max="27" width="12.7109375" customWidth="1"/>
-    <col min="28" max="28" width="29.28515625" customWidth="1"/>
-    <col min="29" max="29" width="20.42578125" customWidth="1"/>
-    <col min="30" max="30" width="36" customWidth="1"/>
-    <col min="31" max="31" width="70.5703125" customWidth="1"/>
-    <col min="32" max="32" width="21.140625" customWidth="1"/>
-    <col min="33" max="33" width="20.28515625" customWidth="1"/>
+    <col min="3" max="3" width="19.5" customWidth="1"/>
+    <col min="5" max="5" width="22.5" customWidth="1"/>
+    <col min="6" max="6" width="23.33203125" customWidth="1"/>
+    <col min="8" max="8" width="25.5" customWidth="1"/>
+    <col min="9" max="9" width="19.6640625" customWidth="1"/>
+    <col min="10" max="11" width="13.5" customWidth="1"/>
+    <col min="12" max="12" width="28.6640625" customWidth="1"/>
+    <col min="13" max="13" width="19.5" customWidth="1"/>
+    <col min="14" max="14" width="12.1640625" customWidth="1"/>
+    <col min="15" max="15" width="13.83203125" customWidth="1"/>
+    <col min="16" max="16" width="17.33203125" customWidth="1"/>
+    <col min="17" max="17" width="36.83203125" style="4" customWidth="1"/>
+    <col min="18" max="18" width="13" customWidth="1"/>
+    <col min="19" max="19" width="22.5" customWidth="1"/>
+    <col min="21" max="21" width="14" customWidth="1"/>
+    <col min="22" max="22" width="15.5" customWidth="1"/>
+    <col min="23" max="23" width="15" customWidth="1"/>
+    <col min="24" max="24" width="21.5" customWidth="1"/>
+    <col min="25" max="25" width="29.1640625" customWidth="1"/>
+    <col min="26" max="26" width="52" customWidth="1"/>
+    <col min="27" max="27" width="47.6640625" style="4" customWidth="1"/>
+    <col min="28" max="28" width="12.6640625" customWidth="1"/>
+    <col min="29" max="29" width="29.33203125" customWidth="1"/>
+    <col min="30" max="30" width="20.5" customWidth="1"/>
+    <col min="31" max="31" width="36" customWidth="1"/>
+    <col min="32" max="32" width="70.5" customWidth="1"/>
+    <col min="33" max="33" width="21.1640625" customWidth="1"/>
+    <col min="34" max="34" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" ht="16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1129,76 +1132,79 @@
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="6" t="s">
+      <c r="AA1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" ht="16">
       <c r="B2" t="s">
         <v>108</v>
       </c>
@@ -1215,54 +1221,54 @@
       <c r="H2" t="s">
         <v>151</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="L2" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>160</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>41</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>125</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>44</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>1</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>33</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>36</v>
       </c>
-      <c r="T2">
+      <c r="U2">
         <v>50</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>107</v>
       </c>
-      <c r="X2" s="10" t="s">
+      <c r="Y2" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="Z2"/>
-      <c r="AB2" s="5" t="s">
+      <c r="AA2"/>
+      <c r="AC2" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="AC2" s="5" t="s">
+      <c r="AD2" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="AD2" s="4" t="s">
+      <c r="AE2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AE2" s="4" t="s">
+      <c r="AF2" s="4" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" ht="48">
       <c r="B3" t="s">
         <v>108</v>
       </c>
@@ -1279,57 +1285,57 @@
       <c r="H3" t="s">
         <v>151</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="L3" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>161</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>42</v>
       </c>
-      <c r="N3" s="9" t="s">
+      <c r="O3" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="P3" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="P3"/>
-      <c r="Q3">
+      <c r="Q3"/>
+      <c r="R3">
         <v>2</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>34</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>36</v>
       </c>
-      <c r="T3">
+      <c r="U3">
         <v>1</v>
       </c>
-      <c r="W3" t="s">
+      <c r="X3" t="s">
         <v>106</v>
       </c>
-      <c r="X3" s="9" t="s">
+      <c r="Y3" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="Z3" t="s">
         <v>50</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AA3" t="s">
         <v>51</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AB3" t="s">
         <v>52</v>
       </c>
-      <c r="AD3" s="4" t="s">
+      <c r="AE3" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="AE3" s="4" t="s">
+      <c r="AF3" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" ht="16">
       <c r="B4" t="s">
         <v>108</v>
       </c>
@@ -1346,42 +1352,42 @@
       <c r="H4" t="s">
         <v>151</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="L4" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>162</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>43</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="O4" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>38</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>3</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>33</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
         <v>39</v>
       </c>
-      <c r="T4">
+      <c r="U4">
         <v>10</v>
       </c>
-      <c r="Z4"/>
-      <c r="AD4" s="4" t="s">
-        <v>54</v>
-      </c>
+      <c r="AA4"/>
       <c r="AE4" s="4" t="s">
         <v>54</v>
       </c>
+      <c r="AF4" s="4" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" ht="16">
       <c r="B5" t="s">
         <v>108</v>
       </c>
@@ -1397,45 +1403,45 @@
       <c r="H5" t="s">
         <v>151</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="L5" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="L5" s="12" t="s">
+      <c r="M5" s="12" t="s">
         <v>163</v>
       </c>
-      <c r="M5" s="12" t="s">
+      <c r="N5" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>124</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>45</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <v>4</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>33</v>
       </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
         <v>36</v>
       </c>
-      <c r="T5">
+      <c r="U5">
         <v>5</v>
       </c>
-      <c r="Z5"/>
-      <c r="AB5" s="5" t="s">
+      <c r="AA5"/>
+      <c r="AC5" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="AD5" t="s">
+      <c r="AE5" t="s">
         <v>55</v>
       </c>
-      <c r="AE5" t="s">
+      <c r="AF5" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="6" spans="1:33" ht="45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:34" ht="51">
       <c r="B6" t="s">
         <v>113</v>
       </c>
@@ -1454,51 +1460,51 @@
       <c r="H6" t="s">
         <v>79</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>122</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>57</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>64</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>109</v>
       </c>
-      <c r="P6" s="4" t="s">
+      <c r="Q6" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <v>1</v>
       </c>
-      <c r="R6" t="s">
+      <c r="S6" t="s">
         <v>33</v>
       </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
         <v>36</v>
       </c>
-      <c r="T6">
+      <c r="U6">
         <v>200</v>
       </c>
-      <c r="X6" s="8"/>
-      <c r="Y6" s="8" t="s">
-        <v>95</v>
-      </c>
+      <c r="Y6" s="8"/>
       <c r="Z6" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AA6" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="AB6" t="s">
         <v>52</v>
       </c>
-      <c r="AD6" s="4" t="s">
+      <c r="AE6" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="AE6" t="s">
+      <c r="AF6" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:33" ht="75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:34" ht="85">
       <c r="B7" t="s">
         <v>115</v>
       </c>
@@ -1517,51 +1523,51 @@
       <c r="H7" t="s">
         <v>80</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="L7" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>140</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>64</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>109</v>
       </c>
-      <c r="P7" s="4" t="s">
+      <c r="Q7" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="Q7">
+      <c r="R7">
         <v>1</v>
       </c>
-      <c r="R7" t="s">
+      <c r="S7" t="s">
         <v>33</v>
       </c>
-      <c r="S7" t="s">
+      <c r="T7" t="s">
         <v>36</v>
       </c>
-      <c r="T7">
+      <c r="U7">
         <v>200</v>
       </c>
-      <c r="X7" s="8"/>
-      <c r="Y7" s="8" t="s">
-        <v>96</v>
-      </c>
+      <c r="Y7" s="8"/>
       <c r="Z7" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="AA7" t="s">
+      <c r="AA7" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="AB7" t="s">
         <v>52</v>
       </c>
-      <c r="AD7" s="4" t="s">
+      <c r="AE7" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="AE7" t="s">
+      <c r="AF7" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:33" ht="75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:34" ht="85">
       <c r="B8" t="s">
         <v>116</v>
       </c>
@@ -1580,51 +1586,51 @@
       <c r="H8" t="s">
         <v>81</v>
       </c>
-      <c r="K8" s="5" t="s">
+      <c r="L8" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>141</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>64</v>
       </c>
-      <c r="N8" t="s">
+      <c r="O8" t="s">
         <v>109</v>
       </c>
-      <c r="P8" s="4" t="s">
+      <c r="Q8" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="Q8">
+      <c r="R8">
         <v>1</v>
       </c>
-      <c r="R8" t="s">
+      <c r="S8" t="s">
         <v>33</v>
       </c>
-      <c r="S8" t="s">
+      <c r="T8" t="s">
         <v>36</v>
       </c>
-      <c r="T8">
+      <c r="U8">
         <v>200</v>
       </c>
-      <c r="X8" s="8"/>
-      <c r="Y8" s="8" t="s">
-        <v>97</v>
-      </c>
+      <c r="Y8" s="8"/>
       <c r="Z8" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="AA8" t="s">
+      <c r="AA8" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="AB8" t="s">
         <v>52</v>
       </c>
-      <c r="AD8" s="4" t="s">
+      <c r="AE8" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="AE8" t="s">
+      <c r="AF8" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:33" ht="60" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:34" ht="68">
       <c r="B9" t="s">
         <v>114</v>
       </c>
@@ -1643,51 +1649,51 @@
       <c r="H9" t="s">
         <v>82</v>
       </c>
-      <c r="K9" s="5" t="s">
+      <c r="L9" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>142</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>64</v>
       </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>109</v>
       </c>
-      <c r="P9" s="4" t="s">
+      <c r="Q9" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="Q9">
+      <c r="R9">
         <v>1</v>
       </c>
-      <c r="R9" t="s">
+      <c r="S9" t="s">
         <v>33</v>
       </c>
-      <c r="S9" t="s">
+      <c r="T9" t="s">
         <v>36</v>
       </c>
-      <c r="T9">
+      <c r="U9">
         <v>200</v>
       </c>
-      <c r="X9" s="8"/>
-      <c r="Y9" s="8" t="s">
-        <v>98</v>
-      </c>
+      <c r="Y9" s="8"/>
       <c r="Z9" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="AA9" t="s">
+      <c r="AA9" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="AB9" t="s">
         <v>52</v>
       </c>
-      <c r="AD9" s="4" t="s">
+      <c r="AE9" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="AE9" t="s">
+      <c r="AF9" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:33" ht="60" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:34" ht="68">
       <c r="B10" t="s">
         <v>110</v>
       </c>
@@ -1706,51 +1712,51 @@
       <c r="H10" t="s">
         <v>83</v>
       </c>
-      <c r="K10" s="5" t="s">
+      <c r="L10" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
         <v>143</v>
       </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
         <v>64</v>
       </c>
-      <c r="N10" t="s">
+      <c r="O10" t="s">
         <v>109</v>
       </c>
-      <c r="P10" s="4" t="s">
+      <c r="Q10" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="Q10">
+      <c r="R10">
         <v>1</v>
       </c>
-      <c r="R10" t="s">
+      <c r="S10" t="s">
         <v>33</v>
       </c>
-      <c r="S10" t="s">
+      <c r="T10" t="s">
         <v>36</v>
       </c>
-      <c r="T10">
+      <c r="U10">
         <v>200</v>
       </c>
-      <c r="X10" s="8"/>
-      <c r="Y10" s="8" t="s">
-        <v>99</v>
-      </c>
+      <c r="Y10" s="8"/>
       <c r="Z10" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="AA10" t="s">
+      <c r="AA10" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="AB10" t="s">
         <v>52</v>
       </c>
-      <c r="AD10" s="4" t="s">
+      <c r="AE10" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="AE10" t="s">
+      <c r="AF10" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:33" ht="30.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:34" ht="33">
       <c r="B11" t="s">
         <v>112</v>
       </c>
@@ -1769,42 +1775,42 @@
       <c r="H11" t="s">
         <v>84</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>111</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>58</v>
       </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
         <v>64</v>
       </c>
-      <c r="N11" t="s">
+      <c r="O11" t="s">
         <v>109</v>
       </c>
-      <c r="P11" s="4" t="s">
+      <c r="Q11" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="Q11">
+      <c r="R11">
         <v>1</v>
       </c>
-      <c r="R11" t="s">
+      <c r="S11" t="s">
         <v>33</v>
       </c>
-      <c r="S11" t="s">
+      <c r="T11" t="s">
         <v>35</v>
       </c>
-      <c r="T11">
+      <c r="U11">
         <v>3</v>
       </c>
-      <c r="Y11" s="7"/>
-      <c r="AD11" s="4" t="s">
+      <c r="Z11" s="7"/>
+      <c r="AE11" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="AE11" t="s">
+      <c r="AF11" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:33" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:34" ht="17">
       <c r="B12" t="s">
         <v>112</v>
       </c>
@@ -1823,49 +1829,49 @@
       <c r="H12" t="s">
         <v>84</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>111</v>
       </c>
-      <c r="L12" t="s">
+      <c r="M12" t="s">
         <v>59</v>
       </c>
-      <c r="M12" t="s">
+      <c r="N12" t="s">
         <v>65</v>
       </c>
-      <c r="N12" t="s">
+      <c r="O12" t="s">
         <v>156</v>
       </c>
-      <c r="P12" s="4" t="s">
+      <c r="Q12" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="Q12">
+      <c r="R12">
         <v>2</v>
       </c>
-      <c r="R12" t="s">
+      <c r="S12" t="s">
         <v>33</v>
       </c>
-      <c r="S12" t="s">
+      <c r="T12" t="s">
         <v>36</v>
       </c>
-      <c r="T12">
+      <c r="U12">
         <v>100</v>
       </c>
-      <c r="V12" s="15"/>
-      <c r="Y12" s="7"/>
-      <c r="AB12" t="s">
+      <c r="W12" s="15"/>
+      <c r="Z12" s="7"/>
+      <c r="AC12" t="s">
         <v>78</v>
       </c>
-      <c r="AC12" t="s">
+      <c r="AD12" t="s">
         <v>104</v>
       </c>
-      <c r="AD12" t="s">
+      <c r="AE12" t="s">
         <v>65</v>
       </c>
-      <c r="AE12" t="s">
+      <c r="AF12" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="13" spans="1:33" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34" ht="16">
       <c r="B13" t="s">
         <v>112</v>
       </c>
@@ -1884,44 +1890,44 @@
       <c r="H13" t="s">
         <v>84</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>111</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>60</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>66</v>
       </c>
-      <c r="N13" t="s">
+      <c r="O13" t="s">
         <v>128</v>
       </c>
-      <c r="P13" s="4" t="s">
+      <c r="Q13" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="Q13">
+      <c r="R13">
         <v>3</v>
       </c>
-      <c r="R13" t="s">
+      <c r="S13" t="s">
         <v>33</v>
       </c>
-      <c r="S13" t="s">
+      <c r="T13" t="s">
         <v>36</v>
       </c>
-      <c r="T13">
+      <c r="U13">
         <v>100</v>
       </c>
-      <c r="AB13" s="4" t="s">
+      <c r="AC13" s="4" t="s">
         <v>102</v>
-      </c>
-      <c r="AD13" t="s">
-        <v>85</v>
       </c>
       <c r="AE13" t="s">
         <v>85</v>
       </c>
+      <c r="AF13" t="s">
+        <v>85</v>
+      </c>
     </row>
-    <row r="14" spans="1:33" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:34" ht="16">
       <c r="B14" t="s">
         <v>112</v>
       </c>
@@ -1940,44 +1946,44 @@
       <c r="H14" t="s">
         <v>84</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>111</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" t="s">
         <v>61</v>
       </c>
-      <c r="M14" t="s">
+      <c r="N14" t="s">
         <v>67</v>
       </c>
-      <c r="N14" t="s">
+      <c r="O14" t="s">
         <v>129</v>
       </c>
-      <c r="P14" s="4" t="s">
+      <c r="Q14" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="Q14">
+      <c r="R14">
         <v>4</v>
       </c>
-      <c r="R14" t="s">
+      <c r="S14" t="s">
         <v>33</v>
       </c>
-      <c r="S14" t="s">
+      <c r="T14" t="s">
         <v>36</v>
       </c>
-      <c r="T14">
+      <c r="U14">
         <v>100</v>
       </c>
-      <c r="AB14" s="4" t="s">
+      <c r="AC14" s="4" t="s">
         <v>101</v>
-      </c>
-      <c r="AD14" t="s">
-        <v>86</v>
       </c>
       <c r="AE14" t="s">
         <v>86</v>
       </c>
+      <c r="AF14" t="s">
+        <v>86</v>
+      </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" ht="16">
       <c r="B15" t="s">
         <v>112</v>
       </c>
@@ -1996,44 +2002,44 @@
       <c r="H15" t="s">
         <v>84</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
         <v>111</v>
       </c>
-      <c r="L15" t="s">
+      <c r="M15" t="s">
         <v>62</v>
       </c>
-      <c r="M15" t="s">
+      <c r="N15" t="s">
         <v>68</v>
       </c>
-      <c r="N15" t="s">
+      <c r="O15" t="s">
         <v>131</v>
       </c>
-      <c r="P15" s="4" t="s">
+      <c r="Q15" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="Q15">
+      <c r="R15">
         <v>5</v>
       </c>
-      <c r="R15" t="s">
+      <c r="S15" t="s">
         <v>33</v>
       </c>
-      <c r="S15" t="s">
+      <c r="T15" t="s">
         <v>35</v>
       </c>
-      <c r="T15">
+      <c r="U15">
         <v>3</v>
       </c>
-      <c r="AB15">
+      <c r="AC15">
         <v>0</v>
-      </c>
-      <c r="AD15" t="s">
-        <v>87</v>
       </c>
       <c r="AE15" t="s">
         <v>87</v>
       </c>
+      <c r="AF15" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34" ht="16">
       <c r="B16" t="s">
         <v>112</v>
       </c>
@@ -2052,45 +2058,45 @@
       <c r="H16" t="s">
         <v>84</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
         <v>111</v>
       </c>
-      <c r="L16" t="s">
+      <c r="M16" t="s">
         <v>63</v>
       </c>
-      <c r="M16" t="s">
+      <c r="N16" t="s">
         <v>69</v>
       </c>
-      <c r="N16" t="s">
+      <c r="O16" t="s">
         <v>130</v>
       </c>
-      <c r="P16" s="4" t="s">
+      <c r="Q16" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="Q16">
+      <c r="R16">
         <v>6</v>
       </c>
-      <c r="R16" t="s">
+      <c r="S16" t="s">
         <v>33</v>
       </c>
-      <c r="S16" t="s">
+      <c r="T16" t="s">
         <v>35</v>
       </c>
-      <c r="T16">
+      <c r="U16">
         <v>3</v>
       </c>
-      <c r="AB16">
+      <c r="AC16">
         <v>100</v>
-      </c>
-      <c r="AD16" t="s">
-        <v>88</v>
       </c>
       <c r="AE16" t="s">
         <v>88</v>
       </c>
+      <c r="AF16" t="s">
+        <v>88</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AG16" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:AH16" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -2104,23 +2110,23 @@
       <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
-    <col min="3" max="3" width="31.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
-    <col min="5" max="6" width="18.28515625" customWidth="1"/>
-    <col min="7" max="7" width="30.140625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="20.42578125" style="4" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" customWidth="1"/>
-    <col min="10" max="10" width="21.28515625" customWidth="1"/>
-    <col min="11" max="11" width="23.7109375" customWidth="1"/>
-    <col min="12" max="13" width="30.140625" style="4" customWidth="1"/>
-    <col min="14" max="14" width="24.42578125" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="3" max="3" width="31.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+    <col min="5" max="6" width="18.33203125" customWidth="1"/>
+    <col min="7" max="7" width="30.1640625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="20.5" style="4" customWidth="1"/>
+    <col min="9" max="9" width="17.5" customWidth="1"/>
+    <col min="10" max="10" width="21.33203125" customWidth="1"/>
+    <col min="11" max="11" width="23.6640625" customWidth="1"/>
+    <col min="12" max="13" width="30.1640625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="14" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="14" customFormat="1" ht="14" customHeight="1">
       <c r="A1" s="13" t="s">
         <v>133</v>
       </c>
@@ -2164,7 +2170,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="16">
       <c r="A2" t="s">
         <v>144</v>
       </c>
@@ -2201,7 +2207,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="16">
       <c r="A3" t="s">
         <v>144</v>
       </c>
@@ -2233,7 +2239,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="48">
       <c r="A4" t="s">
         <v>145</v>
       </c>
@@ -2273,7 +2279,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="16">
       <c r="A5" t="s">
         <v>145</v>
       </c>
@@ -2307,7 +2313,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="16">
       <c r="A6" t="s">
         <v>145</v>
       </c>
@@ -2341,7 +2347,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="16">
       <c r="A7" t="s">
         <v>145</v>
       </c>
@@ -2375,7 +2381,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="16">
       <c r="A8" t="s">
         <v>145</v>
       </c>
@@ -2409,7 +2415,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="225" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="176">
       <c r="A9" t="s">
         <v>145</v>
       </c>

</xml_diff>

<commit_message>
added derivation columns (blank) - QRS_EQ5D-5L
</commit_message>
<xml_diff>
--- a/curation/draft/collection/collection_specialization_QRS_EQ5D-5L.xlsx
+++ b/curation/draft/collection/collection_specialization_QRS_EQ5D-5L.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dagmarkottig/COSMoS/curation/draft/collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86B9646F-2B6B-6B47-950B-E3CA83A9B8AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C29AB9D-CD51-614C-957A-59A594BF5F34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4300" yWindow="780" windowWidth="29900" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="FORM_QRS_EQ5D-5L" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Collection_QRS_EQ5D-5L'!$A$1:$AH$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Collection_QRS_EQ5D-5L'!$A$1:$AJ$16</definedName>
   </definedNames>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="167">
   <si>
     <t>package_date</t>
   </si>
@@ -537,6 +537,12 @@
   </si>
   <si>
     <t>[NOT SUBMITTED]; QSSTAT = NOT DONE</t>
+  </si>
+  <si>
+    <t>derived_variable</t>
+  </si>
+  <si>
+    <t>derivation_description</t>
   </si>
 </sst>
 </file>
@@ -1060,12 +1066,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH16"/>
+  <dimension ref="A1:AJ16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="T1" sqref="T1"/>
-      <selection pane="bottomLeft" activeCell="AF3" sqref="AF3"/>
+      <selection pane="bottomLeft" activeCell="X4" sqref="X4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1086,21 +1092,21 @@
     <col min="19" max="19" width="22.5" customWidth="1"/>
     <col min="21" max="21" width="14" customWidth="1"/>
     <col min="22" max="22" width="15.5" customWidth="1"/>
-    <col min="23" max="23" width="15" customWidth="1"/>
-    <col min="24" max="24" width="21.5" customWidth="1"/>
-    <col min="25" max="25" width="29.1640625" customWidth="1"/>
-    <col min="26" max="26" width="52" customWidth="1"/>
-    <col min="27" max="27" width="47.6640625" style="4" customWidth="1"/>
-    <col min="28" max="28" width="12.6640625" customWidth="1"/>
-    <col min="29" max="29" width="29.33203125" customWidth="1"/>
-    <col min="30" max="30" width="20.5" customWidth="1"/>
-    <col min="31" max="31" width="36" customWidth="1"/>
-    <col min="32" max="32" width="70.5" customWidth="1"/>
-    <col min="33" max="33" width="21.1640625" customWidth="1"/>
-    <col min="34" max="34" width="20.33203125" customWidth="1"/>
+    <col min="23" max="25" width="15" customWidth="1"/>
+    <col min="26" max="26" width="21.5" customWidth="1"/>
+    <col min="27" max="27" width="29.1640625" customWidth="1"/>
+    <col min="28" max="28" width="52" customWidth="1"/>
+    <col min="29" max="29" width="47.6640625" style="4" customWidth="1"/>
+    <col min="30" max="30" width="12.6640625" customWidth="1"/>
+    <col min="31" max="31" width="29.33203125" customWidth="1"/>
+    <col min="32" max="32" width="20.5" customWidth="1"/>
+    <col min="33" max="33" width="36" customWidth="1"/>
+    <col min="34" max="34" width="70.5" customWidth="1"/>
+    <col min="35" max="35" width="21.1640625" customWidth="1"/>
+    <col min="36" max="36" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="16">
+    <row r="1" spans="1:36" ht="16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1171,40 +1177,46 @@
         <v>21</v>
       </c>
       <c r="X1" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="Z1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="6" t="s">
+      <c r="AC1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:34" ht="16">
+    <row r="2" spans="1:36" ht="16">
       <c r="B2" t="s">
         <v>107</v>
       </c>
@@ -1248,27 +1260,27 @@
       <c r="U2">
         <v>50</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Z2" t="s">
         <v>106</v>
       </c>
-      <c r="Y2" s="10" t="s">
+      <c r="AA2" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="AA2"/>
-      <c r="AC2" s="5" t="s">
+      <c r="AC2"/>
+      <c r="AE2" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="AD2" s="5" t="s">
+      <c r="AF2" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="AE2" s="4" t="s">
+      <c r="AG2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AF2" s="4" t="s">
+      <c r="AH2" s="4" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="3" spans="1:34" ht="48">
+    <row r="3" spans="1:36" ht="48">
       <c r="B3" t="s">
         <v>107</v>
       </c>
@@ -1313,29 +1325,29 @@
       <c r="U3">
         <v>1</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Z3" t="s">
         <v>105</v>
       </c>
-      <c r="Y3" s="9" t="s">
+      <c r="AA3" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AB3" t="s">
         <v>50</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AC3" t="s">
         <v>51</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AD3" t="s">
         <v>52</v>
       </c>
-      <c r="AE3" s="4" t="s">
+      <c r="AG3" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="AF3" s="4" t="s">
+      <c r="AH3" s="4" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="4" spans="1:34" ht="16">
+    <row r="4" spans="1:36" ht="16">
       <c r="B4" t="s">
         <v>107</v>
       </c>
@@ -1379,15 +1391,15 @@
       <c r="U4">
         <v>10</v>
       </c>
-      <c r="AA4"/>
-      <c r="AE4" s="4" t="s">
+      <c r="AC4"/>
+      <c r="AG4" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="AF4" s="4" t="s">
+      <c r="AH4" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:34" ht="16">
+    <row r="5" spans="1:36" ht="16">
       <c r="B5" t="s">
         <v>107</v>
       </c>
@@ -1430,18 +1442,18 @@
       <c r="U5">
         <v>5</v>
       </c>
-      <c r="AA5"/>
-      <c r="AC5" s="5" t="s">
+      <c r="AC5"/>
+      <c r="AE5" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="AE5" t="s">
+      <c r="AG5" t="s">
         <v>54</v>
       </c>
-      <c r="AF5" t="s">
+      <c r="AH5" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="6" spans="1:34" ht="51">
+    <row r="6" spans="1:36" ht="51">
       <c r="B6" t="s">
         <v>112</v>
       </c>
@@ -1487,24 +1499,24 @@
       <c r="U6">
         <v>200</v>
       </c>
-      <c r="Y6" s="8"/>
-      <c r="Z6" s="8" t="s">
+      <c r="AA6" s="8"/>
+      <c r="AB6" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="AA6" s="8" t="s">
+      <c r="AC6" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="AB6" t="s">
+      <c r="AD6" t="s">
         <v>52</v>
       </c>
-      <c r="AE6" s="4" t="s">
+      <c r="AG6" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="AF6" t="s">
+      <c r="AH6" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="7" spans="1:34" ht="85">
+    <row r="7" spans="1:36" ht="85">
       <c r="B7" t="s">
         <v>114</v>
       </c>
@@ -1550,24 +1562,24 @@
       <c r="U7">
         <v>200</v>
       </c>
-      <c r="Y7" s="8"/>
-      <c r="Z7" s="8" t="s">
+      <c r="AA7" s="8"/>
+      <c r="AB7" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="AA7" s="8" t="s">
+      <c r="AC7" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="AB7" t="s">
+      <c r="AD7" t="s">
         <v>52</v>
       </c>
-      <c r="AE7" s="4" t="s">
+      <c r="AG7" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="AF7" t="s">
+      <c r="AH7" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:34" ht="85">
+    <row r="8" spans="1:36" ht="85">
       <c r="B8" t="s">
         <v>115</v>
       </c>
@@ -1613,24 +1625,24 @@
       <c r="U8">
         <v>200</v>
       </c>
-      <c r="Y8" s="8"/>
-      <c r="Z8" s="8" t="s">
+      <c r="AA8" s="8"/>
+      <c r="AB8" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="AA8" s="8" t="s">
+      <c r="AC8" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="AB8" t="s">
+      <c r="AD8" t="s">
         <v>52</v>
       </c>
-      <c r="AE8" s="4" t="s">
+      <c r="AG8" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="AF8" t="s">
+      <c r="AH8" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:34" ht="68">
+    <row r="9" spans="1:36" ht="68">
       <c r="B9" t="s">
         <v>113</v>
       </c>
@@ -1676,24 +1688,24 @@
       <c r="U9">
         <v>200</v>
       </c>
-      <c r="Y9" s="8"/>
-      <c r="Z9" s="8" t="s">
+      <c r="AA9" s="8"/>
+      <c r="AB9" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="AA9" s="8" t="s">
+      <c r="AC9" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="AB9" t="s">
+      <c r="AD9" t="s">
         <v>52</v>
       </c>
-      <c r="AE9" s="4" t="s">
+      <c r="AG9" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="AF9" t="s">
+      <c r="AH9" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:34" ht="68">
+    <row r="10" spans="1:36" ht="68">
       <c r="B10" t="s">
         <v>109</v>
       </c>
@@ -1739,24 +1751,24 @@
       <c r="U10">
         <v>200</v>
       </c>
-      <c r="Y10" s="8"/>
-      <c r="Z10" s="8" t="s">
+      <c r="AA10" s="8"/>
+      <c r="AB10" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="AA10" s="8" t="s">
+      <c r="AC10" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="AB10" t="s">
+      <c r="AD10" t="s">
         <v>52</v>
       </c>
-      <c r="AE10" s="4" t="s">
+      <c r="AG10" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="AF10" t="s">
+      <c r="AH10" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="11" spans="1:34" ht="33">
+    <row r="11" spans="1:36" ht="33">
       <c r="B11" t="s">
         <v>111</v>
       </c>
@@ -1802,15 +1814,15 @@
       <c r="U11">
         <v>3</v>
       </c>
-      <c r="Z11" s="7"/>
-      <c r="AE11" s="4" t="s">
+      <c r="AB11" s="7"/>
+      <c r="AG11" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="AF11" t="s">
+      <c r="AH11" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:34" ht="17">
+    <row r="12" spans="1:36" ht="17">
       <c r="B12" t="s">
         <v>111</v>
       </c>
@@ -1857,21 +1869,23 @@
         <v>100</v>
       </c>
       <c r="W12" s="15"/>
-      <c r="Z12" s="7"/>
-      <c r="AC12" t="s">
+      <c r="X12" s="15"/>
+      <c r="Y12" s="15"/>
+      <c r="AB12" s="7"/>
+      <c r="AE12" t="s">
         <v>77</v>
       </c>
-      <c r="AD12" t="s">
+      <c r="AF12" t="s">
         <v>103</v>
       </c>
-      <c r="AE12" t="s">
+      <c r="AG12" t="s">
         <v>64</v>
       </c>
-      <c r="AF12" t="s">
+      <c r="AH12" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="13" spans="1:34" ht="16">
+    <row r="13" spans="1:36" ht="16">
       <c r="B13" t="s">
         <v>111</v>
       </c>
@@ -1917,17 +1931,17 @@
       <c r="U13">
         <v>100</v>
       </c>
-      <c r="AC13" s="4" t="s">
+      <c r="AE13" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="AE13" t="s">
+      <c r="AG13" t="s">
         <v>84</v>
       </c>
-      <c r="AF13" t="s">
+      <c r="AH13" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:34" ht="16">
+    <row r="14" spans="1:36" ht="16">
       <c r="B14" t="s">
         <v>111</v>
       </c>
@@ -1973,17 +1987,17 @@
       <c r="U14">
         <v>100</v>
       </c>
-      <c r="AC14" s="4" t="s">
+      <c r="AE14" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="AE14" t="s">
+      <c r="AG14" t="s">
         <v>85</v>
       </c>
-      <c r="AF14" t="s">
+      <c r="AH14" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:34" ht="16">
+    <row r="15" spans="1:36" ht="16">
       <c r="B15" t="s">
         <v>111</v>
       </c>
@@ -2029,17 +2043,17 @@
       <c r="U15">
         <v>3</v>
       </c>
-      <c r="AC15">
+      <c r="AE15">
         <v>0</v>
       </c>
-      <c r="AE15" t="s">
+      <c r="AG15" t="s">
         <v>86</v>
       </c>
-      <c r="AF15" t="s">
+      <c r="AH15" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="16" spans="1:34" ht="16">
+    <row r="16" spans="1:36" ht="16">
       <c r="B16" t="s">
         <v>111</v>
       </c>
@@ -2085,18 +2099,18 @@
       <c r="U16">
         <v>3</v>
       </c>
-      <c r="AC16">
+      <c r="AE16">
         <v>100</v>
       </c>
-      <c r="AE16" t="s">
+      <c r="AG16" t="s">
         <v>87</v>
       </c>
-      <c r="AF16" t="s">
+      <c r="AH16" t="s">
         <v>87</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AH16" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:AJ16" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>